<commit_message>
correction for fill blank on float/int columns
</commit_message>
<xml_diff>
--- a/data/processed/duplicate-dates.xlsx
+++ b/data/processed/duplicate-dates.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ds_projects\maven-challenge\Maven-Power-Outage-Challenge\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB65910-B2DF-4B82-AA74-011A0D7E2DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817E629B-33DF-4AA7-B6C1-7A12114696F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$209</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -50,18 +47,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -91,13 +82,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,13 +392,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -417,423 +405,423 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>37937.708333333343</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>37937.708333333343</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>37937.708333333343</v>
+      <c r="A7" s="2">
+        <v>38174.25</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>37959.354166666657</v>
+      <c r="A8" s="2">
+        <v>38174.25</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>37959.354166666657</v>
+      <c r="A9" s="2">
+        <v>44673.666666666657</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>38128.083333333343</v>
+      <c r="A10" s="2">
+        <v>44673.666666666657</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>38128.083333333343</v>
+      <c r="A11" s="2">
+        <v>38593.298611111109</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>38135.5</v>
+      <c r="A12" s="2">
+        <v>38593.298611111109</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>38135.5</v>
+      <c r="A13" s="2">
+        <v>38760.083333333343</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>38135.5</v>
+      <c r="A14" s="2">
+        <v>38760.083333333343</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>38174.25</v>
+      <c r="A15" s="2">
+        <v>38922.606249999997</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>38174.25</v>
+      <c r="A16" s="2">
+        <v>38922.606249999997</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>38593.298611111109</v>
+      <c r="A17" s="2">
+        <v>39005.29791666667</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>38593.298611111109</v>
+      <c r="A18" s="2">
+        <v>39005.29791666667</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>38760.083333333343</v>
+      <c r="A19" s="2">
+        <v>39343.21875</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>38760.083333333343</v>
+      <c r="A20" s="2">
+        <v>39381.280555555553</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>38922.606249999997</v>
+      <c r="A21" s="2">
+        <v>39381.280555555553</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>38922.606249999997</v>
+      <c r="A22" s="2">
+        <v>39488.166666666657</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>39005.29791666667</v>
+      <c r="A23" s="2">
+        <v>39488.458333333343</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>39005.29791666667</v>
+      <c r="A24" s="2">
+        <v>39488.458333333343</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>39343.21875</v>
+      <c r="A25" s="2">
+        <v>39504.54791666667</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>39343.21875</v>
+      <c r="A26" s="2">
+        <v>39504.54791666667</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>39381.280555555553</v>
+      <c r="A27" s="2">
+        <v>39504.54791666667</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>39381.280555555553</v>
+      <c r="A28" s="2">
+        <v>39504.54791666667</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>39488.166666666657</v>
+      <c r="A29" s="2">
+        <v>44243.041666666657</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>39488.166666666657</v>
+      <c r="A30" s="2">
+        <v>44243.041666666657</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>39488.458333333343</v>
+      <c r="A31" s="2">
+        <v>44243.041666666657</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>39488.458333333343</v>
+      <c r="A32" s="2">
+        <v>44243.732638888891</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>39504.54791666667</v>
+      <c r="A33" s="2">
+        <v>44243.732638888891</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>39504.54791666667</v>
+      <c r="A34" s="2">
+        <v>44242.416666666657</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>39504.54791666667</v>
+      <c r="A35" s="2">
+        <v>44242.416666666657</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>39504.54791666667</v>
+      <c r="A36" s="2">
+        <v>39651.125</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>39651.125</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>39651.125</v>
+      <c r="A38" s="2">
+        <v>39703.76458333333</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>39703.76458333333</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
-        <v>39703.76458333333</v>
+      <c r="A40" s="2">
+        <v>44047.5</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>40388.777083333327</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>40388.777083333327</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>40392.458333333343</v>
+      <c r="A46" s="2">
+        <v>43770.033333333333</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>40392.458333333343</v>
+      <c r="A47" s="2">
+        <v>43770.033333333333</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>40392.458333333343</v>
+      <c r="A48" s="2">
+        <v>40478.166666666657</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
-        <v>40392.458333333343</v>
+      <c r="A49" s="2">
+        <v>40660.416666666657</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>40478.166666666657</v>
+      <c r="A50" s="2">
+        <v>43383.25</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>40478.166666666657</v>
+      <c r="A51" s="2">
+        <v>43383.25</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>40637.000694444447</v>
+        <v>40735.375</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>40637.000694444447</v>
+        <v>40735.375</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>40660.416666666657</v>
+        <v>43161.5</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>40660.416666666657</v>
+        <v>40783.000694444447</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>40735.375</v>
+        <v>43116.541666666657</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>40735.375</v>
+        <v>43116.541666666657</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>40783.000694444447</v>
+        <v>40845.374305555553</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>40783.000694444447</v>
+        <v>40845.374305555553</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>40783.000694444447</v>
+        <v>40877.416666666657</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>40845.374305555553</v>
+        <v>42972.708333333343</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>40845.374305555553</v>
+        <v>42972.708333333343</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>40877.416666666657</v>
+        <v>41089.666666666657</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>40877.416666666657</v>
+        <v>41089.666666666657</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>41089.666666666657</v>
+        <v>41206</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>41089.666666666657</v>
+        <v>41206</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>41206</v>
+        <v>41211.375</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>41206</v>
+        <v>41211.375</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>41211.375</v>
+        <v>41211.5</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>41211.375</v>
+        <v>41211.666666666657</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>41211.458333333343</v>
+        <v>41211.666666666657</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>41211.458333333343</v>
+        <v>41211.666666666657</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>41211.5</v>
+        <v>42365.708333333343</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>41211.5</v>
+        <v>41621.458333333343</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>41211.666666666657</v>
+        <v>41621.458333333343</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>41211.666666666657</v>
+        <v>41645.826388888891</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>41211.666666666657</v>
+        <v>41645.826388888891</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>41621.458333333343</v>
+        <v>41645.826388888891</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>41621.458333333343</v>
+        <v>41645.826388888891</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>41645.826388888891</v>
+        <v>41646.25</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>41645.826388888891</v>
+        <v>41646.25</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>41645.826388888891</v>
+        <v>42011.357638888891</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>41645.826388888891</v>
+        <v>42011.357638888891</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>41646.25</v>
+        <v>41828.729166666657</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>41646.25</v>
+        <v>41828.729166666657</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
@@ -848,182 +836,182 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>41828.729166666657</v>
+        <v>42336.25</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>41828.729166666657</v>
+        <v>42336.25</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>42011.357638888891</v>
+        <v>42365.708333333343</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>42011.357638888891</v>
+        <v>42570.65625</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>42336.25</v>
+        <v>42570.65625</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>42336.25</v>
+        <v>41211.5</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>42365.708333333343</v>
+        <v>41211.458333333343</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>42365.708333333343</v>
+        <v>41211.458333333343</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>42570.65625</v>
+        <v>42883.8125</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>42570.65625</v>
+        <v>42883.8125</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>42883.8125</v>
+        <v>42938.916666666657</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>42883.8125</v>
+        <v>42938.916666666657</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>42938.916666666657</v>
+        <v>43034.345138888893</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>42938.916666666657</v>
+        <v>43034.345138888893</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>42972.708333333343</v>
+        <v>40877.416666666657</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>42972.708333333343</v>
+        <v>43118.208333333343</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>43034.345138888893</v>
+        <v>43118.208333333343</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>43034.345138888893</v>
+        <v>43159.505555555559</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>43116.541666666657</v>
+        <v>43159.505555555559</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>43116.541666666657</v>
+        <v>40783.000694444447</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>43118.208333333343</v>
+        <v>40783.000694444447</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>43118.208333333343</v>
+        <v>43161.5</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>43159.505555555559</v>
+        <v>43319.056944444441</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>43159.505555555559</v>
+        <v>43319.056944444441</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>43161.5</v>
+        <v>43358.625</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>43161.5</v>
+        <v>43358.625</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>43319.056944444441</v>
+        <v>40660.416666666657</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>43319.056944444441</v>
+        <v>43477.479166666657</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>43358.625</v>
+        <v>43477.479166666657</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>43358.625</v>
+        <v>40637.000694444447</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>43383.25</v>
+        <v>40637.000694444447</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>43383.25</v>
+        <v>43556.285416666673</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>43477.479166666657</v>
+        <v>43556.285416666673</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>43477.479166666657</v>
+        <v>40478.166666666657</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>43556.285416666673</v>
+        <v>40392.458333333343</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>43556.285416666673</v>
+        <v>43761.03402777778</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
@@ -1033,17 +1021,17 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>43761.03402777778</v>
+        <v>40392.458333333343</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>43770.033333333333</v>
+        <v>40392.458333333343</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>43770.033333333333</v>
+        <v>40392.458333333343</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
@@ -1093,7 +1081,7 @@
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>44047.5</v>
+        <v>44062.583333333343</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
@@ -1103,7 +1091,7 @@
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>44062.583333333343</v>
+        <v>44070.504166666673</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
@@ -1113,7 +1101,7 @@
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>44070.504166666673</v>
+        <v>44241.354166666657</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
@@ -1123,7 +1111,7 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>44241.354166666657</v>
+        <v>44242</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
@@ -1133,7 +1121,7 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>44242</v>
+        <v>44242.055555555547</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
@@ -1143,7 +1131,7 @@
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>44242.055555555547</v>
+        <v>44242.07916666667</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
@@ -1153,7 +1141,7 @@
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>44242.07916666667</v>
+        <v>44242.23333333333</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
@@ -1163,277 +1151,277 @@
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>44242.23333333333</v>
+        <v>44242.416666666657</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>44242.416666666657</v>
+        <v>44242.75</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>44242.416666666657</v>
+        <v>44242.75</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>44242.416666666657</v>
+        <v>44242.75</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>44242.75</v>
+        <v>44243.041666666657</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>44242.75</v>
+        <v>44243.283333333333</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>44242.75</v>
+        <v>44243.283333333333</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>44243.041666666657</v>
+        <v>44244.708333333343</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>44243.041666666657</v>
+        <v>44244.708333333343</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>44243.041666666657</v>
+        <v>44244.75</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>44243.041666666657</v>
+        <v>44244.75</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>44243.283333333333</v>
+        <v>39488.166666666657</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>44243.283333333333</v>
+        <v>44387.020833333343</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>44243.732638888891</v>
+        <v>44387.020833333343</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>44243.732638888891</v>
+        <v>39343.21875</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>44244.708333333343</v>
+        <v>44455.617361111108</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>44244.708333333343</v>
+        <v>44455.617361111108</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>44244.75</v>
+        <v>44474.479861111111</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>44244.75</v>
+        <v>44474.479861111111</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>44387.020833333343</v>
+        <v>44545.833333333343</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>44387.020833333343</v>
+        <v>44545.833333333343</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>44455.617361111108</v>
+        <v>44562.525000000001</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>44455.617361111108</v>
+        <v>44562.525000000001</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>44474.479861111111</v>
+        <v>44595.538888888892</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>44474.479861111111</v>
+        <v>44595.538888888892</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>44545.833333333343</v>
+        <v>44661.65347222222</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>44545.833333333343</v>
+        <v>44661.65347222222</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>44562.525000000001</v>
+        <v>44662.856249999997</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>44562.525000000001</v>
+        <v>44662.856249999997</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>44595.538888888892</v>
+        <v>44690.684027777781</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>44595.538888888892</v>
+        <v>44690.684027777781</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>44661.65347222222</v>
+        <v>44693.623611111107</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>44661.65347222222</v>
+        <v>44693.623611111107</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>44662.856249999997</v>
+        <v>44696.875</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>44662.856249999997</v>
+        <v>44696.875</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>44673.666666666657</v>
+        <v>44720.041666666657</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>44673.666666666657</v>
+        <v>44720.041666666657</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>44690.684027777781</v>
+        <v>44761.654166666667</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>44690.684027777781</v>
+        <v>44761.654166666667</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>44693.623611111107</v>
+        <v>44782.508333333331</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>44693.623611111107</v>
+        <v>44782.508333333331</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>44696.875</v>
+        <v>44798.040972222218</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>44696.875</v>
+        <v>44798.040972222218</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>44720.041666666657</v>
+        <v>44832.625</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>44720.041666666657</v>
+        <v>44832.625</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>44761.654166666667</v>
+        <v>38135.5</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>44761.654166666667</v>
+        <v>38135.5</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>44782.508333333331</v>
+        <v>38135.5</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>44782.508333333331</v>
+        <v>38128.083333333343</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>44798.040972222218</v>
+        <v>38128.083333333343</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>44798.040972222218</v>
+        <v>44901</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>44832.625</v>
+        <v>44901</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>44832.625</v>
+        <v>37959.354166666657</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>44901</v>
+        <v>37959.354166666657</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>44901</v>
+        <v>37937.708333333343</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
@@ -1457,11 +1445,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A209" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A209">
-      <sortCondition ref="A1:A209"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
review of missing data
</commit_message>
<xml_diff>
--- a/data/processed/duplicate-dates.xlsx
+++ b/data/processed/duplicate-dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ds_projects\maven-challenge\Maven-Power-Outage-Challenge\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A348B168-EEE3-4B8A-A65D-CCA42275571F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CE6FE7-1EB6-43D7-AF93-668ADFD59FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35235" yWindow="75" windowWidth="21960" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -91,18 +91,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -410,13 +407,13 @@
   <dimension ref="A1:A209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -425,1042 +422,1042 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>37847.673611111109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>37937.708333333343</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>37937.708333333343</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>37937.708333333343</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>37959.354166666657</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>37959.354166666657</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>38128.083333333343</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>38128.083333333343</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>38135.5</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>38135.5</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>38135.5</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>38174.25</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>38174.25</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>38593.298611111109</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>38593.298611111109</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>38760.083333333343</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>38760.083333333343</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>38922.606249999997</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>38922.606249999997</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>39005.29791666667</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>39005.29791666667</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>39343.21875</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>39343.21875</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>39381.280555555553</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>39381.280555555553</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>39488.166666666657</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>39488.166666666657</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>39488.458333333343</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>39488.458333333343</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>39504.54791666667</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>39504.54791666667</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>39504.54791666667</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>39504.54791666667</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>39651.125</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>39651.125</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>39703.76458333333</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>39703.76458333333</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="3">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="3">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="3">
         <v>40346.395833333343</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="3">
         <v>40388.777083333327</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>40388.777083333327</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="3">
         <v>40392.458333333343</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="3">
         <v>40392.458333333343</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="3">
         <v>40392.458333333343</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="3">
         <v>40392.458333333343</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="3">
         <v>40478.166666666657</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="3">
         <v>40478.166666666657</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="3">
         <v>40637.000694444447</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="3">
         <v>40637.000694444447</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="3">
         <v>40660.416666666657</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="3">
         <v>40660.416666666657</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="3">
         <v>40735.375</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="3">
         <v>40735.375</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="3">
         <v>40783.000694444447</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="3">
         <v>40783.000694444447</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="3">
         <v>40783.000694444447</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="3">
         <v>40845.374305555553</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="3">
         <v>40845.374305555553</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="3">
         <v>40877.416666666657</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="3">
         <v>40877.416666666657</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="A65" s="3">
         <v>41089.666666666657</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="3">
         <v>41089.666666666657</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="3">
         <v>41206</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="3">
         <v>41206</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="3">
         <v>41211.375</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="3">
         <v>41211.375</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="3">
         <v>41211.458333333343</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="3">
         <v>41211.458333333343</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="3">
         <v>41211.5</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="3">
         <v>41211.5</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="3">
         <v>41211.666666666657</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="3">
         <v>41211.666666666657</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="3">
         <v>41211.666666666657</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="3">
         <v>41621.458333333343</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="3">
         <v>41621.458333333343</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="3">
         <v>41645.826388888891</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="3">
         <v>41645.826388888891</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="3">
         <v>41645.826388888891</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="3">
         <v>41645.826388888891</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="3">
         <v>41646.25</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="3">
         <v>41646.25</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="A86" s="3">
         <v>41646.375</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="3">
         <v>41646.375</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="3">
         <v>41828.729166666657</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="3">
         <v>41828.729166666657</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="3">
         <v>42011.357638888891</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="3">
         <v>42011.357638888891</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="3">
         <v>42336.25</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="3">
         <v>42336.25</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="3">
         <v>42365.708333333343</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="3">
         <v>42365.708333333343</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="3">
         <v>42570.65625</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="3">
         <v>42570.65625</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="3">
         <v>42883.8125</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="3">
         <v>42883.8125</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="3">
         <v>42938.916666666657</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="3">
         <v>42938.916666666657</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="3">
         <v>42972.708333333343</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="3">
         <v>42972.708333333343</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="3">
         <v>43034.345138888893</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="3">
         <v>43034.345138888893</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="3">
         <v>43116.541666666657</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="2">
+      <c r="A107" s="3">
         <v>43116.541666666657</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="3">
         <v>43118.208333333343</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="3">
         <v>43118.208333333343</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="3">
         <v>43159.505555555559</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="3">
         <v>43159.505555555559</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="3">
         <v>43161.5</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="3">
         <v>43161.5</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="3">
         <v>43319.056944444441</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="3">
         <v>43319.056944444441</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="3">
         <v>43358.625</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="3">
         <v>43358.625</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="3">
         <v>43383.25</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="3">
         <v>43383.25</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="3">
         <v>43477.479166666657</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="3">
         <v>43477.479166666657</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="3">
         <v>43556.285416666673</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="A123" s="3">
         <v>43556.285416666673</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="A124" s="3">
         <v>43761.03402777778</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="A125" s="3">
         <v>43761.03402777778</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="A126" s="3">
         <v>43770.033333333333</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="A127" s="3">
         <v>43770.033333333333</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="A128" s="3">
         <v>43791</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="2">
+      <c r="A129" s="3">
         <v>43791</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="2">
+      <c r="A130" s="3">
         <v>43839.963194444441</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="2">
+      <c r="A131" s="3">
         <v>43839.963194444441</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="2">
+      <c r="A132" s="3">
         <v>43906.333333333343</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="2">
+      <c r="A133" s="3">
         <v>43906.333333333343</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="2">
+      <c r="A134" s="3">
         <v>43917.54583333333</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="2">
+      <c r="A135" s="3">
         <v>43917.54583333333</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="2">
+      <c r="A136" s="3">
         <v>44047.5</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="2">
+      <c r="A137" s="3">
         <v>44047.5</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="2">
+      <c r="A138" s="3">
         <v>44062.583333333343</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="2">
+      <c r="A139" s="3">
         <v>44062.583333333343</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="2">
+      <c r="A140" s="3">
         <v>44070.504166666673</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="2">
+      <c r="A141" s="3">
         <v>44070.504166666673</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="2">
+      <c r="A142" s="3">
         <v>44241.354166666657</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="2">
+      <c r="A143" s="3">
         <v>44241.354166666657</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="2">
+      <c r="A144" s="3">
         <v>44242</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="2">
+      <c r="A145" s="3">
         <v>44242</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="2">
+      <c r="A146" s="3">
         <v>44242.055555555547</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="2">
+      <c r="A147" s="3">
         <v>44242.055555555547</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="2">
+      <c r="A148" s="3">
         <v>44242.07916666667</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="2">
+      <c r="A149" s="3">
         <v>44242.07916666667</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="2">
+      <c r="A150" s="3">
         <v>44242.23333333333</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="2">
+      <c r="A151" s="3">
         <v>44242.23333333333</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="2">
+      <c r="A152" s="3">
         <v>44242.416666666657</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="2">
+      <c r="A153" s="3">
         <v>44242.416666666657</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="2">
+      <c r="A154" s="3">
         <v>44242.416666666657</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="2">
+      <c r="A155" s="3">
         <v>44242.75</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="2">
+      <c r="A156" s="3">
         <v>44242.75</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="2">
+      <c r="A157" s="3">
         <v>44242.75</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="2">
+      <c r="A158" s="3">
         <v>44243.041666666657</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="2">
+      <c r="A159" s="3">
         <v>44243.041666666657</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="2">
+      <c r="A160" s="3">
         <v>44243.041666666657</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="2">
+      <c r="A161" s="3">
         <v>44243.041666666657</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="2">
+      <c r="A162" s="3">
         <v>44243.283333333333</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="2">
+      <c r="A163" s="3">
         <v>44243.283333333333</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="2">
+      <c r="A164" s="3">
         <v>44243.732638888891</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="2">
+      <c r="A165" s="3">
         <v>44243.732638888891</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="2">
+      <c r="A166" s="3">
         <v>44244.708333333343</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="2">
+      <c r="A167" s="3">
         <v>44244.708333333343</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="2">
+      <c r="A168" s="3">
         <v>44244.75</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="2">
+      <c r="A169" s="3">
         <v>44244.75</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="2">
+      <c r="A170" s="3">
         <v>44387.020833333343</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="2">
+      <c r="A171" s="3">
         <v>44387.020833333343</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="2">
+      <c r="A172" s="3">
         <v>44455.617361111108</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="2">
+      <c r="A173" s="3">
         <v>44455.617361111108</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="2">
+      <c r="A174" s="3">
         <v>44474.479861111111</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="2">
+      <c r="A175" s="3">
         <v>44474.479861111111</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="2">
+      <c r="A176" s="3">
         <v>44545.833333333343</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="2">
+      <c r="A177" s="3">
         <v>44545.833333333343</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="2">
+      <c r="A178" s="3">
         <v>44562.525000000001</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="2">
+      <c r="A179" s="3">
         <v>44562.525000000001</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="2">
+      <c r="A180" s="3">
         <v>44595.538888888892</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="2">
+      <c r="A181" s="3">
         <v>44595.538888888892</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A182" s="2">
+      <c r="A182" s="3">
         <v>44661.65347222222</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="2">
+      <c r="A183" s="3">
         <v>44661.65347222222</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A184" s="2">
+      <c r="A184" s="3">
         <v>44662.856249999997</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="2">
+      <c r="A185" s="3">
         <v>44662.856249999997</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="2">
+      <c r="A186" s="3">
         <v>44673.666666666657</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="2">
+      <c r="A187" s="3">
         <v>44673.666666666657</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
+      <c r="A188" s="3">
         <v>44690.684027777781</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="2">
+      <c r="A189" s="3">
         <v>44690.684027777781</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="2">
+      <c r="A190" s="3">
         <v>44693.623611111107</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A191" s="2">
+      <c r="A191" s="3">
         <v>44693.623611111107</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="2">
+      <c r="A192" s="3">
         <v>44696.875</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="2">
+      <c r="A193" s="3">
         <v>44696.875</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="2">
+      <c r="A194" s="3">
         <v>44720.041666666657</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="2">
+      <c r="A195" s="3">
         <v>44720.041666666657</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="2">
+      <c r="A196" s="3">
         <v>44761.654166666667</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="2">
+      <c r="A197" s="3">
         <v>44761.654166666667</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="2">
+      <c r="A198" s="3">
         <v>44782.508333333331</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="2">
+      <c r="A199" s="3">
         <v>44782.508333333331</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="2">
+      <c r="A200" s="3">
         <v>44798.040972222218</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="2">
+      <c r="A201" s="3">
         <v>44798.040972222218</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="2">
+      <c r="A202" s="3">
         <v>44832.625</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="2">
+      <c r="A203" s="3">
         <v>44832.625</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="2">
+      <c r="A204" s="3">
         <v>44901</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="2">
+      <c r="A205" s="3">
         <v>44901</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="2">
+      <c r="A206" s="3">
         <v>44988.652777777781</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="2">
+      <c r="A207" s="3">
         <v>44988.652777777781</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="2">
+      <c r="A208" s="3">
         <v>44989.295138888891</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="2">
+      <c r="A209" s="3">
         <v>44989.295138888891</v>
       </c>
     </row>

</xml_diff>